<commit_message>
adding images as scatter points
</commit_message>
<xml_diff>
--- a/Resources/sportsref_fourfactors.xlsx
+++ b/Resources/sportsref_fourfactors.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99584ccd66595d1f/Documents/mathletics/NBA practice/nba21analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{033DFF0F-49CB-4D09-9B3F-ACC2443E344E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{033DFF0F-49CB-4D09-9B3F-ACC2443E344E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4197C738-2DC9-4A96-BDC6-F9FD8D06404F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$AB$31</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -286,7 +289,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1129,14 +1132,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
@@ -1243,7 +1246,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>2848</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1587,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2619,7 +2622,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2791,7 +2794,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2963,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3049,7 +3052,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3135,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3221,7 +3224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3307,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="12.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3651,7 +3654,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3737,7 +3740,7 @@
         <v>3557</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3823,8 +3826,6 @@
         <v>3181</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>